<commit_message>
updated for adding MGT6753
</commit_message>
<xml_diff>
--- a/GTMSA_course_list.xlsx
+++ b/GTMSA_course_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchingchen/Documents/ching870423/usa_master/MTA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F58556-3408-B149-9675-650A5C53EEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F8672C-9F92-7541-A4BB-C604C9DBC9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FD8F2A78-D165-5445-ACDF-D30981A5BD45}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FD8F2A78-D165-5445-ACDF-D30981A5BD45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>waivable introductory</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>ISYE8813THO</t>
+  </si>
+  <si>
+    <t>MGT6753</t>
   </si>
 </sst>
 </file>
@@ -308,11 +311,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7223DEDF-F2CC-694B-A1DB-4CD510A0E65D}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D75" sqref="D1:D75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -703,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -714,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -725,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -736,18 +738,18 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -759,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -771,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -779,11 +781,11 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -791,11 +793,11 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -805,8 +807,8 @@
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
+      <c r="C15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -816,8 +818,8 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
+      <c r="C16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -827,8 +829,8 @@
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>25</v>
+      <c r="C17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -838,8 +840,8 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>26</v>
+      <c r="C18" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -849,8 +851,8 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>27</v>
+      <c r="C19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -860,8 +862,8 @@
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>28</v>
+      <c r="C20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -871,8 +873,8 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
+      <c r="C21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -882,8 +884,8 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>30</v>
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -891,10 +893,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -904,8 +906,8 @@
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>32</v>
+      <c r="C24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -915,8 +917,8 @@
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>33</v>
+      <c r="C25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -926,8 +928,8 @@
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>34</v>
+      <c r="C26" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -937,8 +939,8 @@
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>35</v>
+      <c r="C27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,19 +950,19 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>36</v>
+      <c r="C28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>21</v>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -968,11 +970,11 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>19</v>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -980,11 +982,11 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>37</v>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -994,8 +996,8 @@
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>38</v>
+      <c r="C32" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1005,8 +1007,8 @@
       <c r="B33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>39</v>
+      <c r="C33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1016,8 +1018,8 @@
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>40</v>
+      <c r="C34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,8 +1029,8 @@
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>41</v>
+      <c r="C35" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1038,8 +1040,8 @@
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>42</v>
+      <c r="C36" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1049,8 +1051,8 @@
       <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>43</v>
+      <c r="C37" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1060,8 +1062,8 @@
       <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>44</v>
+      <c r="C38" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1071,8 +1073,8 @@
       <c r="B39" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>45</v>
+      <c r="C39" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1082,8 +1084,8 @@
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>46</v>
+      <c r="C40" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1093,19 +1095,19 @@
       <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>47</v>
+      <c r="C41" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>18</v>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
       </c>
       <c r="H42" s="2"/>
     </row>
@@ -1113,11 +1115,11 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>48</v>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1127,8 +1129,8 @@
       <c r="B44" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>49</v>
+      <c r="C44" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1138,8 +1140,8 @@
       <c r="B45" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>50</v>
+      <c r="C45" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1149,19 +1151,19 @@
       <c r="B46" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>51</v>
+      <c r="C46" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>20</v>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
       </c>
       <c r="H47" s="2"/>
     </row>
@@ -1169,11 +1171,11 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>64</v>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H48" s="1"/>
     </row>
@@ -1181,11 +1183,11 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>19</v>
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="H49" s="2"/>
     </row>
@@ -1197,7 +1199,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H50" s="2"/>
     </row>
@@ -1205,11 +1207,11 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>52</v>
+      <c r="C51" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1219,8 +1221,8 @@
       <c r="B52" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>53</v>
+      <c r="C52" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1231,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1242,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1253,18 +1255,18 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="s">
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="H56" s="2"/>
     </row>
@@ -1272,11 +1274,11 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -1284,10 +1286,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -1298,7 +1300,7 @@
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -1309,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1320,7 +1322,7 @@
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -1331,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -1342,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -1353,7 +1355,7 @@
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -1364,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -1375,7 +1377,7 @@
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -1386,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -1394,10 +1396,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -1408,7 +1410,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -1419,7 +1421,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -1430,7 +1432,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -1441,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -1452,7 +1454,7 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -1463,20 +1465,31 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
+        <v>74</v>
+      </c>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>